<commit_message>
added National Directory Profiles
</commit_message>
<xml_diff>
--- a/output/CodeSystem-AcceptingPatientsCS.xlsx
+++ b/output/CodeSystem-AcceptingPatientsCS.xlsx
@@ -24,7 +24,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/national-directory-query/CodeSystem/AcceptingPatientsCS</t>
+    <t>http://hl7.org/fhir/us/fhir-directory-query/CodeSystem/AcceptingPatientsCS</t>
   </si>
   <si>
     <t>Version</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2021-12-16T11:05:58-05:00</t>
+    <t>2021-12-17T13:53:37-05:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>